<commit_message>
Moved footprint/model for USB-C connector to local library. Updated BOM. Updated images. Regenerated gerber/drill files.
</commit_message>
<xml_diff>
--- a/hd44780_tutorial_BOM.xlsx
+++ b/hd44780_tutorial_BOM.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prj\youtube\ian_ward\LCD2004_HD44780_Tutorial\HD44780 Tutorial PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prj\yt\ian_ward\hd44780_tutorial\HD44780-tutorial-PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{57521302-469E-4E05-A859-4F1CAA1D646E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5D1AE01A-710E-49D0-AD36-81800A3D3E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="13952"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="13952" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="hd44780_tutorial" sheetId="1" r:id="rId1"/>
+    <sheet name="hd44780_tutorial_BOM" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="108">
   <si>
     <t>#</t>
   </si>
@@ -64,9 +64,6 @@
     <t>D3</t>
   </si>
   <si>
-    <t>LED_BAR_GRAPH  8_SEG_SOCKET</t>
-  </si>
-  <si>
     <t>footprints:LED_Bar_Graph_8_SEG_SOCKET</t>
   </si>
   <si>
@@ -103,21 +100,12 @@
     <t>J2</t>
   </si>
   <si>
-    <t>USB4105-GF-A</t>
-  </si>
-  <si>
-    <t>footprints:USB_C_Receptacle_HRO_TYPE-C-31-M-12</t>
-  </si>
-  <si>
     <t>R1, R5, R6, R9</t>
   </si>
   <si>
     <t>Resistor_THT:R_Axial_DIN0207_L6.3mm_D2.5mm_P7.62mm_Horizontal</t>
   </si>
   <si>
-    <t>R2, R3</t>
-  </si>
-  <si>
     <t>R7, R8</t>
   </si>
   <si>
@@ -166,20 +154,6 @@
     <t>footprints:SW_DS02C-254-1L-08BE</t>
   </si>
   <si>
-    <r>
-      <t>330</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ω</t>
-    </r>
-  </si>
-  <si>
     <t>1KΩ</t>
   </si>
   <si>
@@ -195,16 +169,187 @@
     <t>Datasheet</t>
   </si>
   <si>
-    <t>Digikey</t>
-  </si>
-  <si>
     <t>Vendor URL</t>
+  </si>
+  <si>
+    <t>UJC-HP-3-SMT-TR</t>
+  </si>
+  <si>
+    <t>R2, R3, R4</t>
+  </si>
+  <si>
+    <t>RN2</t>
+  </si>
+  <si>
+    <t>footprints:CUI_UJC-HP-3-SMT-TR</t>
+  </si>
+  <si>
+    <t>330Ω</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8_SEG_LED  BAR_GRAPH (RED)</t>
+  </si>
+  <si>
+    <t>Generic</t>
+  </si>
+  <si>
+    <t>KiCad</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/tdk-corporation/FG28C0G1H103JNT06/5803088</t>
+  </si>
+  <si>
+    <t>https://product.tdk.com/en/system/files?file=dam/doc/product/capacitor/ceramic/lead-mlcc/catalog/leadmlcc_halogenfree_fg_en.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cui-devices/UJC-HP-M-G-5-MSMT-TR/16629543</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/ujc-hp-m-g-5-msmt-tr.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/4609X-101-471LF/3593678</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/3386P-1-502LF/1088535</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/e-switch/TL2230EEF140/4029358</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/te-connectivity-alcoswitch-switches/1825967-1/1632540</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cui-devices/DS02C-254-1L-08BE/11310898</t>
+  </si>
+  <si>
+    <t>https://www.bourns.com/docs/Product-Datasheets/4600x.pdf</t>
+  </si>
+  <si>
+    <t>https://www.bourns.com/docs/Product-Datasheets/3386.pdf</t>
+  </si>
+  <si>
+    <t>https://eswitch.wpengine.com/wp-content/uploads/2022/06/TL2201-3.pdf</t>
+  </si>
+  <si>
+    <t>https://www.te.com/usa-en/product-1825967-1.datasheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/ds02-254.pdf</t>
+  </si>
+  <si>
+    <t>Vendor\Part #</t>
+  </si>
+  <si>
+    <t>Digikey\445-173474-1-ND</t>
+  </si>
+  <si>
+    <t>Digikey\2223-UJC-HP-M-G-5-MSMT-TRDKR-ND</t>
+  </si>
+  <si>
+    <t>Digikey\4609X-101-471LF-ND</t>
+  </si>
+  <si>
+    <t>Digikey\3386P-1-502LF</t>
+  </si>
+  <si>
+    <t>Digikey\EG6031-ND</t>
+  </si>
+  <si>
+    <t>Digikey\450-1654-ND</t>
+  </si>
+  <si>
+    <t>Digikey\2223-DS02C-254-1L-08BE-ND</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Unpolarized capacitor</t>
+  </si>
+  <si>
+    <t>LED\3mm\Yellow</t>
+  </si>
+  <si>
+    <t>LED\3mm\Green</t>
+  </si>
+  <si>
+    <t>LED\3mm\Blue</t>
+  </si>
+  <si>
+    <t>LED\3mm\Red</t>
+  </si>
+  <si>
+    <t>LED Bar Graph\Red\1x8</t>
+  </si>
+  <si>
+    <t>M2.5</t>
+  </si>
+  <si>
+    <t>Female Pin Header\1x16\2.54mm pitch</t>
+  </si>
+  <si>
+    <t>Type C, 20 VDC, 3A, Horizontal, Power Only</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/MFR-25FRF52-330R/9139001</t>
+  </si>
+  <si>
+    <t>https://www.yageo.com/upload/media/product/app/datasheet/lr/yageo-mfr_datasheet.pdf</t>
+  </si>
+  <si>
+    <t>Digikey\13-MFR-25FRF52-330RCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/MFR-25FTE52-1K/9139842</t>
+  </si>
+  <si>
+    <t>Digikey\13-MFR-25FTE52-1KCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/MFR-25FTE52-5K1/9140307</t>
+  </si>
+  <si>
+    <t>Digikey\13-MFR-25FTE52-5K1CT-ND</t>
+  </si>
+  <si>
+    <t>Resistor\5K1 Ohm\1%\1/4W\Axial</t>
+  </si>
+  <si>
+    <t>Resistor\330 Ohm\1%\1/4W\Axial</t>
+  </si>
+  <si>
+    <t>Resistor\1K Ohm\1%\1/4W\Axial</t>
+  </si>
+  <si>
+    <t>Digikey\4609X-101-102LF-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/4609X-101-102LF/3593658</t>
+  </si>
+  <si>
+    <t>Resistor Array\ 8 Resistors\1K Ohm\9SIP</t>
+  </si>
+  <si>
+    <t>Resistor Array\ 8 Resistors\470 Ohm\9SIP</t>
+  </si>
+  <si>
+    <t>Trimmer Pot\5 kOhms\0.5W\1/2W\Through Hole</t>
+  </si>
+  <si>
+    <t>Switch\Pushbutton\DPDT\Through Hole</t>
+  </si>
+  <si>
+    <t>Switch\Tactile\SPST-NO\0.05A\24V\Through Hole</t>
+  </si>
+  <si>
+    <t>Switch\Piano\8-DIP\SPST\0.025A\24V\Through Hole</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -347,12 +492,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFC000"/>
@@ -366,6 +505,11 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -714,19 +858,24 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1102,56 +1251,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9747EA74-8FD8-4BB9-901B-62A1BA268C81}">
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="1"/>
-    <col min="4" max="4" width="44.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="67.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.25" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="8.25" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.875" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="44.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="89.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="117.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="14.3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="F1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1160,356 +1316,537 @@
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="F2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="F3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="F4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="F6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="F7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="4">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="1">
+      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="4">
         <v>4</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="D11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="4">
         <v>1</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="14.3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="D14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="4">
         <v>1</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="14.3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="1">
-        <v>4</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="F15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C16" s="4">
         <v>2</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="1">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="14.3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="F16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C17" s="4">
         <v>1</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="14.3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="1">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="F17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="14.3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="C18" s="4">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="1">
+      <c r="E18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="4">
         <v>1</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="14.3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="F19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="4">
         <v>1</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="14.3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="14.3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="F20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F10" r:id="rId1"/>
-    <hyperlink ref="G10" r:id="rId2"/>
-    <hyperlink ref="F14" r:id="rId3"/>
-    <hyperlink ref="G14" r:id="rId4"/>
-    <hyperlink ref="F15" r:id="rId5"/>
-    <hyperlink ref="G15" r:id="rId6"/>
-    <hyperlink ref="F16" r:id="rId7"/>
-    <hyperlink ref="G16" r:id="rId8"/>
-    <hyperlink ref="F17" r:id="rId9"/>
-    <hyperlink ref="G17" r:id="rId10"/>
-    <hyperlink ref="F18" r:id="rId11"/>
-    <hyperlink ref="G18" r:id="rId12"/>
-    <hyperlink ref="F19" r:id="rId13"/>
-    <hyperlink ref="G19" r:id="rId14"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated XLSX BOM and README.md
</commit_message>
<xml_diff>
--- a/hd44780_tutorial_BOM.xlsx
+++ b/hd44780_tutorial_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prj\yt\ian_ward\hd44780_tutorial\HD44780-tutorial-PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4434DAEF-E0FB-445F-813B-7754BA0BD068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5439A07-0D4D-4BA9-971B-612470BD1FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="13952" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,27 +154,12 @@
     <t>footprints:SW_DS02C-254-1L-08BE</t>
   </si>
   <si>
-    <t>1KΩ</t>
-  </si>
-  <si>
-    <t>5.1KΩ</t>
-  </si>
-  <si>
-    <t>470Ω</t>
-  </si>
-  <si>
-    <t>5KΩ</t>
-  </si>
-  <si>
     <t>Datasheet</t>
   </si>
   <si>
     <t>Vendor URL</t>
   </si>
   <si>
-    <t>UJC-HP-3-SMT-TR</t>
-  </si>
-  <si>
     <t>R2, R3, R4</t>
   </si>
   <si>
@@ -184,9 +169,6 @@
     <t>footprints:CUI_UJC-HP-3-SMT-TR</t>
   </si>
   <si>
-    <t>330Ω</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 8_SEG_LED  BAR_GRAPH (RED)</t>
   </si>
   <si>
@@ -313,37 +295,55 @@
     <t>Digikey\13-MFR-25FTE52-5K1CT-ND</t>
   </si>
   <si>
-    <t>Resistor\5K1 Ohm\1%\1/4W\Axial</t>
-  </si>
-  <si>
-    <t>Resistor\330 Ohm\1%\1/4W\Axial</t>
-  </si>
-  <si>
-    <t>Resistor\1K Ohm\1%\1/4W\Axial</t>
-  </si>
-  <si>
     <t>Digikey\4609X-101-102LF-ND</t>
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/bourns-inc/4609X-101-102LF/3593658</t>
   </si>
   <si>
-    <t>Resistor Array\ 8 Resistors\1K Ohm\9SIP</t>
-  </si>
-  <si>
-    <t>Resistor Array\ 8 Resistors\470 Ohm\9SIP</t>
-  </si>
-  <si>
-    <t>Trimmer Pot\5 kOhms\0.5W\1/2W\Through Hole</t>
-  </si>
-  <si>
     <t>Switch\Pushbutton\DPDT\Through Hole</t>
   </si>
   <si>
     <t>Switch\Tactile\SPST-NO\0.05A\24V\Through Hole</t>
   </si>
   <si>
-    <t>Switch\Piano\8-DIP\SPST\0.025A\24V\Through Hole</t>
+    <t>UJC-HP-M-G-5-MSMT-TR</t>
+  </si>
+  <si>
+    <t>330ohm</t>
+  </si>
+  <si>
+    <t>1Kohm</t>
+  </si>
+  <si>
+    <t>5.1Kohm</t>
+  </si>
+  <si>
+    <t>470ohm</t>
+  </si>
+  <si>
+    <t>5Kohm</t>
+  </si>
+  <si>
+    <t>Switch\Piano\8-DIP\SPST\0.025mA\24V\Through Hole</t>
+  </si>
+  <si>
+    <t>Trimmer Pot\5kohms\0.5W\1/2W\Through Hole</t>
+  </si>
+  <si>
+    <t>Resistor Array\ 8 Resistors\470ohm\9SIP</t>
+  </si>
+  <si>
+    <t>Resistor Array\ 8 Resistors\1Kohm\9SIP</t>
+  </si>
+  <si>
+    <t>Resistor\5K1ohm\1%\1/4W\Axial</t>
+  </si>
+  <si>
+    <t>Resistor\1Kohm\1%\1/4W\Axial</t>
+  </si>
+  <si>
+    <t>Resistor\330ohm\1%\1/4W\Axial</t>
   </si>
 </sst>
 </file>
@@ -860,7 +860,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -874,7 +874,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="42" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1254,7 +1253,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1287,16 +1286,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1316,16 +1315,16 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>58</v>
+        <v>67</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1345,12 +1344,12 @@
         <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1370,12 +1369,12 @@
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1389,18 +1388,18 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1420,12 +1419,12 @@
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1445,12 +1444,12 @@
         <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1470,12 +1469,12 @@
         <v>21</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1495,12 +1494,12 @@
         <v>24</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1514,22 +1513,22 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1543,22 +1542,22 @@
         <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1566,28 +1565,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C12" s="4">
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1601,22 +1600,22 @@
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1630,19 +1629,19 @@
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>103</v>
@@ -1653,28 +1652,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C15" s="4">
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1688,22 +1687,22 @@
         <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1723,16 +1722,16 @@
         <v>35</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1752,16 +1751,16 @@
         <v>38</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1781,16 +1780,16 @@
         <v>38</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1810,16 +1809,16 @@
         <v>43</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>